<commit_message>
npc data 파싱 605개 배열
</commit_message>
<xml_diff>
--- a/Assets/Database/S_NPCdatabase_Yes.xlsx
+++ b/Assets/Database/S_NPCdatabase_Yes.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACDE6F2-F036-4530-BE01-7A0C381BD31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9E5BAF-EE47-403E-B3D4-1157632E953E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7B594B15-E6F7-40E3-8C22-7C42F4F971ED}"/>
+    <workbookView xWindow="3444" yWindow="204" windowWidth="17280" windowHeight="11772" xr2:uid="{7B594B15-E6F7-40E3-8C22-7C42F4F971ED}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="NPC_01" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -2168,7 +2168,7 @@
   <dimension ref="A1:F606"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="19.2" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
NPCdatabase_Object_Type NPC(심학규 이외 모든 npc) / PLAYER(심학규)
</commit_message>
<xml_diff>
--- a/Assets/Database/S_NPCdatabase_Yes.xlsx
+++ b/Assets/Database/S_NPCdatabase_Yes.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9E5BAF-EE47-403E-B3D4-1157632E953E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6200A0-CCB8-4AB5-864A-DF5AE8BAE034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3444" yWindow="204" windowWidth="17280" windowHeight="11772" xr2:uid="{7B594B15-E6F7-40E3-8C22-7C42F4F971ED}"/>
   </bookViews>
   <sheets>
     <sheet name="NPC_01" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NPC_01!$A$1:$F$606</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="504">
   <si>
     <t>NPC</t>
   </si>
@@ -1724,6 +1727,14 @@
   </si>
   <si>
     <t>뭐 살 것 있소?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLAYER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLAYER</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2168,7 +2179,7 @@
   <dimension ref="A1:F606"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="19.2" x14ac:dyDescent="0.4"/>
@@ -2587,7 +2598,7 @@
         <v>5020</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>150</v>
@@ -3307,7 +3318,7 @@
         <v>5099</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>150</v>
@@ -4447,7 +4458,7 @@
         <v>5218</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>150</v>
@@ -5767,7 +5778,7 @@
         <v>5365</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>150</v>
@@ -5787,7 +5798,7 @@
         <v>5366</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>150</v>
@@ -6547,7 +6558,7 @@
         <v>5440</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>150</v>
@@ -6587,7 +6598,7 @@
         <v>5442</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>150</v>
@@ -6907,7 +6918,7 @@
         <v>5476</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>150</v>
@@ -6967,7 +6978,7 @@
         <v>5479</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>150</v>
@@ -7027,7 +7038,7 @@
         <v>5482</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>150</v>
@@ -7047,7 +7058,7 @@
         <v>5483</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>150</v>
@@ -7107,7 +7118,7 @@
         <v>5486</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>150</v>
@@ -7127,7 +7138,7 @@
         <v>5487</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>150</v>
@@ -7507,7 +7518,7 @@
         <v>5716</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C267" s="2" t="s">
         <v>150</v>
@@ -7847,7 +7858,7 @@
         <v>5733</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C284" s="2" t="s">
         <v>150</v>
@@ -8027,7 +8038,7 @@
         <v>5742</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C293" s="2" t="s">
         <v>150</v>
@@ -9167,7 +9178,7 @@
         <v>5799</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C350" s="2" t="s">
         <v>150</v>
@@ -10427,7 +10438,7 @@
         <v>7001</v>
       </c>
       <c r="B413" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>150</v>
@@ -10447,7 +10458,7 @@
         <v>7002</v>
       </c>
       <c r="B414" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>150</v>
@@ -10467,7 +10478,7 @@
         <v>7003</v>
       </c>
       <c r="B415" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>150</v>
@@ -10507,7 +10518,7 @@
         <v>7005</v>
       </c>
       <c r="B417" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>150</v>
@@ -10527,7 +10538,7 @@
         <v>7006</v>
       </c>
       <c r="B418" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>150</v>
@@ -10547,7 +10558,7 @@
         <v>7007</v>
       </c>
       <c r="B419" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>150</v>
@@ -10567,7 +10578,7 @@
         <v>7008</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>150</v>
@@ -10587,7 +10598,7 @@
         <v>7009</v>
       </c>
       <c r="B421" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>150</v>
@@ -10607,7 +10618,7 @@
         <v>7010</v>
       </c>
       <c r="B422" s="2" t="s">
-        <v>80</v>
+        <v>503</v>
       </c>
       <c r="C422" s="2" t="s">
         <v>150</v>
@@ -10627,7 +10638,7 @@
         <v>7011</v>
       </c>
       <c r="B423" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>150</v>
@@ -10647,7 +10658,7 @@
         <v>7012</v>
       </c>
       <c r="B424" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>150</v>
@@ -10667,7 +10678,7 @@
         <v>7013</v>
       </c>
       <c r="B425" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>150</v>
@@ -10687,7 +10698,7 @@
         <v>7014</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>150</v>
@@ -10707,7 +10718,7 @@
         <v>7015</v>
       </c>
       <c r="B427" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>150</v>
@@ -10727,7 +10738,7 @@
         <v>7016</v>
       </c>
       <c r="B428" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C428" s="2" t="s">
         <v>150</v>
@@ -10767,7 +10778,7 @@
         <v>7018</v>
       </c>
       <c r="B430" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>150</v>
@@ -10787,7 +10798,7 @@
         <v>7019</v>
       </c>
       <c r="B431" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>150</v>
@@ -10807,7 +10818,7 @@
         <v>7020</v>
       </c>
       <c r="B432" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>150</v>
@@ -10827,7 +10838,7 @@
         <v>7021</v>
       </c>
       <c r="B433" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>150</v>
@@ -10847,7 +10858,7 @@
         <v>7022</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>150</v>
@@ -10867,7 +10878,7 @@
         <v>7023</v>
       </c>
       <c r="B435" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C435" s="2" t="s">
         <v>150</v>
@@ -10887,7 +10898,7 @@
         <v>7024</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>150</v>
@@ -10907,7 +10918,7 @@
         <v>7025</v>
       </c>
       <c r="B437" s="2" t="s">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="C437" s="2" t="s">
         <v>150</v>
@@ -10947,7 +10958,7 @@
         <v>7027</v>
       </c>
       <c r="B439" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C439" s="5" t="s">
         <v>338</v>
@@ -11007,7 +11018,7 @@
         <v>7030</v>
       </c>
       <c r="B442" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C442" s="5" t="s">
         <v>338</v>
@@ -11027,7 +11038,7 @@
         <v>7031</v>
       </c>
       <c r="B443" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C443" s="5" t="s">
         <v>338</v>
@@ -11047,7 +11058,7 @@
         <v>7032</v>
       </c>
       <c r="B444" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C444" s="5" t="s">
         <v>338</v>
@@ -11067,7 +11078,7 @@
         <v>7033</v>
       </c>
       <c r="B445" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C445" s="5" t="s">
         <v>338</v>
@@ -11087,7 +11098,7 @@
         <v>7034</v>
       </c>
       <c r="B446" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C446" s="5" t="s">
         <v>338</v>
@@ -11127,7 +11138,7 @@
         <v>7036</v>
       </c>
       <c r="B448" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C448" s="5" t="s">
         <v>338</v>
@@ -11187,7 +11198,7 @@
         <v>7039</v>
       </c>
       <c r="B451" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C451" s="5" t="s">
         <v>338</v>
@@ -11207,7 +11218,7 @@
         <v>7040</v>
       </c>
       <c r="B452" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C452" s="5" t="s">
         <v>338</v>
@@ -11227,7 +11238,7 @@
         <v>7041</v>
       </c>
       <c r="B453" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C453" s="5" t="s">
         <v>338</v>
@@ -11247,7 +11258,7 @@
         <v>7042</v>
       </c>
       <c r="B454" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C454" s="5" t="s">
         <v>338</v>
@@ -11287,7 +11298,7 @@
         <v>7044</v>
       </c>
       <c r="B456" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C456" s="2" t="s">
         <v>338</v>
@@ -11307,7 +11318,7 @@
         <v>7045</v>
       </c>
       <c r="B457" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>338</v>
@@ -11327,7 +11338,7 @@
         <v>7046</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>338</v>
@@ -11347,7 +11358,7 @@
         <v>7047</v>
       </c>
       <c r="B459" s="2" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>338</v>
@@ -11367,7 +11378,7 @@
         <v>7048</v>
       </c>
       <c r="B460" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C460" s="5" t="s">
         <v>338</v>
@@ -11387,7 +11398,7 @@
         <v>7049</v>
       </c>
       <c r="B461" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C461" s="5" t="s">
         <v>338</v>
@@ -11407,7 +11418,7 @@
         <v>7050</v>
       </c>
       <c r="B462" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C462" s="5" t="s">
         <v>338</v>
@@ -11427,7 +11438,7 @@
         <v>7051</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C463" s="5" t="s">
         <v>338</v>
@@ -11447,7 +11458,7 @@
         <v>7052</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C464" s="5" t="s">
         <v>338</v>
@@ -11487,7 +11498,7 @@
         <v>7054</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C466" s="5" t="s">
         <v>338</v>
@@ -11527,7 +11538,7 @@
         <v>7056</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C468" s="5" t="s">
         <v>338</v>
@@ -11587,7 +11598,7 @@
         <v>7059</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C471" s="5" t="s">
         <v>338</v>
@@ -11607,7 +11618,7 @@
         <v>7060</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C472" s="5" t="s">
         <v>338</v>
@@ -11707,7 +11718,7 @@
         <v>7065</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C477" s="5" t="s">
         <v>338</v>
@@ -11727,7 +11738,7 @@
         <v>7066</v>
       </c>
       <c r="B478" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C478" s="5" t="s">
         <v>338</v>
@@ -11747,7 +11758,7 @@
         <v>7067</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C479" s="5" t="s">
         <v>338</v>
@@ -11767,7 +11778,7 @@
         <v>7068</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C480" s="5" t="s">
         <v>338</v>
@@ -11807,7 +11818,7 @@
         <v>7070</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C482" s="5" t="s">
         <v>338</v>
@@ -11887,7 +11898,7 @@
         <v>7074</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C486" s="5" t="s">
         <v>338</v>
@@ -11907,7 +11918,7 @@
         <v>7075</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C487" s="5" t="s">
         <v>338</v>
@@ -12007,7 +12018,7 @@
         <v>7080</v>
       </c>
       <c r="B492" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C492" s="5" t="s">
         <v>338</v>
@@ -12027,7 +12038,7 @@
         <v>7081</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C493" s="5" t="s">
         <v>338</v>
@@ -12047,7 +12058,7 @@
         <v>7082</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C494" s="5" t="s">
         <v>338</v>
@@ -12067,7 +12078,7 @@
         <v>7083</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C495" s="5" t="s">
         <v>338</v>
@@ -12107,7 +12118,7 @@
         <v>7085</v>
       </c>
       <c r="B497" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C497" s="5" t="s">
         <v>338</v>
@@ -12127,7 +12138,7 @@
         <v>7086</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C498" s="5" t="s">
         <v>338</v>
@@ -12147,7 +12158,7 @@
         <v>7087</v>
       </c>
       <c r="B499" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C499" s="5" t="s">
         <v>338</v>
@@ -12167,7 +12178,7 @@
         <v>7088</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C500" s="5" t="s">
         <v>338</v>
@@ -12227,7 +12238,7 @@
         <v>7091</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C503" s="5" t="s">
         <v>338</v>
@@ -12247,7 +12258,7 @@
         <v>7092</v>
       </c>
       <c r="B504" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C504" s="5" t="s">
         <v>338</v>
@@ -12267,7 +12278,7 @@
         <v>7093</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C505" s="5" t="s">
         <v>338</v>
@@ -12287,7 +12298,7 @@
         <v>7094</v>
       </c>
       <c r="B506" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C506" s="5" t="s">
         <v>338</v>
@@ -12467,7 +12478,7 @@
         <v>7103</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C515" s="5" t="s">
         <v>338</v>
@@ -12487,7 +12498,7 @@
         <v>7104</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C516" s="5" t="s">
         <v>338</v>
@@ -12507,7 +12518,7 @@
         <v>7105</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C517" s="5" t="s">
         <v>338</v>
@@ -12527,7 +12538,7 @@
         <v>7106</v>
       </c>
       <c r="B518" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C518" s="5" t="s">
         <v>338</v>
@@ -12547,7 +12558,7 @@
         <v>7107</v>
       </c>
       <c r="B519" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C519" s="5" t="s">
         <v>338</v>
@@ -12567,7 +12578,7 @@
         <v>7108</v>
       </c>
       <c r="B520" s="5" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C520" s="5" t="s">
         <v>338</v>
@@ -12587,7 +12598,7 @@
         <v>7109</v>
       </c>
       <c r="B521" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C521" s="7" t="s">
         <v>338</v>
@@ -12607,7 +12618,7 @@
         <v>7110</v>
       </c>
       <c r="B522" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C522" s="7" t="s">
         <v>338</v>
@@ -12627,7 +12638,7 @@
         <v>7111</v>
       </c>
       <c r="B523" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C523" s="7" t="s">
         <v>338</v>
@@ -12647,7 +12658,7 @@
         <v>7112</v>
       </c>
       <c r="B524" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C524" s="7" t="s">
         <v>338</v>
@@ -12667,7 +12678,7 @@
         <v>7113</v>
       </c>
       <c r="B525" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C525" s="7" t="s">
         <v>338</v>
@@ -12687,7 +12698,7 @@
         <v>7114</v>
       </c>
       <c r="B526" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C526" s="7" t="s">
         <v>338</v>
@@ -12707,7 +12718,7 @@
         <v>7115</v>
       </c>
       <c r="B527" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C527" s="7" t="s">
         <v>338</v>
@@ -12727,7 +12738,7 @@
         <v>7116</v>
       </c>
       <c r="B528" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C528" s="7" t="s">
         <v>338</v>
@@ -12747,7 +12758,7 @@
         <v>7117</v>
       </c>
       <c r="B529" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C529" s="7" t="s">
         <v>338</v>
@@ -12767,7 +12778,7 @@
         <v>7118</v>
       </c>
       <c r="B530" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C530" s="7" t="s">
         <v>338</v>
@@ -12787,7 +12798,7 @@
         <v>7119</v>
       </c>
       <c r="B531" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C531" s="7" t="s">
         <v>338</v>
@@ -12807,7 +12818,7 @@
         <v>7120</v>
       </c>
       <c r="B532" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C532" s="7" t="s">
         <v>338</v>
@@ -12827,7 +12838,7 @@
         <v>7121</v>
       </c>
       <c r="B533" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C533" s="7" t="s">
         <v>338</v>
@@ -12847,7 +12858,7 @@
         <v>7122</v>
       </c>
       <c r="B534" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C534" s="7" t="s">
         <v>338</v>
@@ -12867,7 +12878,7 @@
         <v>7123</v>
       </c>
       <c r="B535" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C535" s="7" t="s">
         <v>338</v>
@@ -12887,7 +12898,7 @@
         <v>7124</v>
       </c>
       <c r="B536" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C536" s="7" t="s">
         <v>338</v>
@@ -12907,7 +12918,7 @@
         <v>7125</v>
       </c>
       <c r="B537" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C537" s="7" t="s">
         <v>338</v>
@@ -12927,7 +12938,7 @@
         <v>7126</v>
       </c>
       <c r="B538" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C538" s="7" t="s">
         <v>338</v>
@@ -12947,7 +12958,7 @@
         <v>7127</v>
       </c>
       <c r="B539" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C539" s="7" t="s">
         <v>338</v>
@@ -12967,7 +12978,7 @@
         <v>7128</v>
       </c>
       <c r="B540" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C540" s="7" t="s">
         <v>338</v>
@@ -12987,7 +12998,7 @@
         <v>7129</v>
       </c>
       <c r="B541" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C541" s="7" t="s">
         <v>338</v>
@@ -13007,7 +13018,7 @@
         <v>7130</v>
       </c>
       <c r="B542" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C542" s="7" t="s">
         <v>338</v>
@@ -13027,7 +13038,7 @@
         <v>7131</v>
       </c>
       <c r="B543" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C543" s="7" t="s">
         <v>338</v>
@@ -13047,7 +13058,7 @@
         <v>7132</v>
       </c>
       <c r="B544" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C544" s="7" t="s">
         <v>338</v>
@@ -13067,7 +13078,7 @@
         <v>7133</v>
       </c>
       <c r="B545" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C545" s="7" t="s">
         <v>338</v>
@@ -13087,7 +13098,7 @@
         <v>7134</v>
       </c>
       <c r="B546" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C546" s="7" t="s">
         <v>338</v>
@@ -13107,7 +13118,7 @@
         <v>7135</v>
       </c>
       <c r="B547" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C547" s="7" t="s">
         <v>338</v>
@@ -13127,7 +13138,7 @@
         <v>7136</v>
       </c>
       <c r="B548" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C548" s="7" t="s">
         <v>338</v>
@@ -13147,7 +13158,7 @@
         <v>7137</v>
       </c>
       <c r="B549" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C549" s="7" t="s">
         <v>338</v>
@@ -13167,7 +13178,7 @@
         <v>7138</v>
       </c>
       <c r="B550" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C550" s="7" t="s">
         <v>338</v>
@@ -13187,7 +13198,7 @@
         <v>7139</v>
       </c>
       <c r="B551" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C551" s="7" t="s">
         <v>338</v>
@@ -13207,7 +13218,7 @@
         <v>7140</v>
       </c>
       <c r="B552" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C552" s="7" t="s">
         <v>338</v>
@@ -13227,7 +13238,7 @@
         <v>7141</v>
       </c>
       <c r="B553" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C553" s="7" t="s">
         <v>338</v>
@@ -13247,7 +13258,7 @@
         <v>7142</v>
       </c>
       <c r="B554" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C554" s="7" t="s">
         <v>338</v>
@@ -13267,7 +13278,7 @@
         <v>7143</v>
       </c>
       <c r="B555" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C555" s="7" t="s">
         <v>338</v>
@@ -13287,7 +13298,7 @@
         <v>7144</v>
       </c>
       <c r="B556" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C556" s="7" t="s">
         <v>338</v>
@@ -13307,7 +13318,7 @@
         <v>7145</v>
       </c>
       <c r="B557" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C557" s="7" t="s">
         <v>338</v>
@@ -13327,7 +13338,7 @@
         <v>7146</v>
       </c>
       <c r="B558" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C558" s="7" t="s">
         <v>338</v>
@@ -13347,7 +13358,7 @@
         <v>7147</v>
       </c>
       <c r="B559" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C559" s="7" t="s">
         <v>338</v>
@@ -13367,7 +13378,7 @@
         <v>7148</v>
       </c>
       <c r="B560" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C560" s="7" t="s">
         <v>338</v>
@@ -13387,7 +13398,7 @@
         <v>7149</v>
       </c>
       <c r="B561" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C561" s="7" t="s">
         <v>338</v>
@@ -13407,7 +13418,7 @@
         <v>7150</v>
       </c>
       <c r="B562" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C562" s="7" t="s">
         <v>338</v>
@@ -13427,7 +13438,7 @@
         <v>7151</v>
       </c>
       <c r="B563" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C563" s="7" t="s">
         <v>338</v>
@@ -13447,7 +13458,7 @@
         <v>7152</v>
       </c>
       <c r="B564" s="7" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C564" s="7" t="s">
         <v>338</v>
@@ -14287,7 +14298,7 @@
         <v>7194</v>
       </c>
       <c r="B606" s="6" t="s">
-        <v>0</v>
+        <v>503</v>
       </c>
       <c r="C606" s="6" t="s">
         <v>338</v>
@@ -14303,6 +14314,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F606" xr:uid="{389FB4EF-C25C-4758-9727-D38BE4993E17}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>